<commit_message>
feat: Add azkaroftadeh and bazmandeh csvs
</commit_message>
<xml_diff>
--- a/projection/csv/bazneshaste_bimepardaz_just_all.xlsx
+++ b/projection/csv/bazneshaste_bimepardaz_just_all.xlsx
@@ -928,7 +928,7 @@
         <v>100297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1">
         <v>70</v>
       </c>
@@ -942,7 +942,7 @@
         <v>56496</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1">
         <v>71</v>
       </c>
@@ -956,7 +956,7 @@
         <v>56496</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1">
         <v>72</v>
       </c>
@@ -970,7 +970,7 @@
         <v>56496</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1">
         <v>73</v>
       </c>
@@ -984,7 +984,7 @@
         <v>56496</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1">
         <v>74</v>
       </c>
@@ -998,7 +998,7 @@
         <v>56496</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1">
         <v>75</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>91806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1">
         <v>76</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>91806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1">
         <v>77</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>91806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1">
         <v>78</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>91806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1">
         <v>79</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>91806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1">
         <v>80</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>18477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1">
         <v>81</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>18477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1">
         <v>82</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>18477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1">
         <v>83</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>18477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1">
         <v>84</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>18477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1">
         <v>85</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>13814</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1">
         <v>86</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>13814</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1">
         <v>87</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>13814</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1">
         <v>88</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>13814</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1">
         <v>89</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>13814</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1">
         <v>90</v>
       </c>

</xml_diff>